<commit_message>
feat: Add ESP-01S header to PCB v0.5
</commit_message>
<xml_diff>
--- a/PCB/teensy-pins.xlsx
+++ b/PCB/teensy-pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ZXTeensy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\git\ZXTeensyIF1\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE37EC-EA34-429E-BA88-9C9692F0AF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4DA617-4A59-4DD2-B760-D86BFC1BB8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34215" yWindow="7650" windowWidth="29010" windowHeight="25500" xr2:uid="{76CCDF92-9EEA-4BF3-89AD-18FB6AC2FABF}"/>
+    <workbookView xWindow="17070" yWindow="2385" windowWidth="29010" windowHeight="25500" xr2:uid="{76CCDF92-9EEA-4BF3-89AD-18FB6AC2FABF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,13 +433,13 @@
     <t>^DataEn</t>
   </si>
   <si>
-    <t>NC_B</t>
-  </si>
-  <si>
     <t>INPUT</t>
   </si>
   <si>
-    <t>NC_A</t>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>TX</t>
   </si>
 </sst>
 </file>
@@ -929,7 +929,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="1">
         <v>28</v>
@@ -1548,70 +1548,70 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="B38" s="1">
         <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="B39" s="1">
         <v>35</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B40" s="1">
         <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="B41" s="1">
         <v>37</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Introduce hardware Serial8 as MB03+ UART
</commit_message>
<xml_diff>
--- a/PCB/teensy-pins.xlsx
+++ b/PCB/teensy-pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\git\ZXTeensyIF1\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4DA617-4A59-4DD2-B760-D86BFC1BB8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B248C06-E0E3-4CC1-8472-050F81B52313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17070" yWindow="2385" windowWidth="29010" windowHeight="25500" xr2:uid="{76CCDF92-9EEA-4BF3-89AD-18FB6AC2FABF}"/>
+    <workbookView xWindow="20760" yWindow="2355" windowWidth="29010" windowHeight="25500" xr2:uid="{76CCDF92-9EEA-4BF3-89AD-18FB6AC2FABF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,13 +433,13 @@
     <t>^DataEn</t>
   </si>
   <si>
-    <t>INPUT</t>
-  </si>
-  <si>
     <t>RX</t>
   </si>
   <si>
     <t>TX</t>
+  </si>
+  <si>
+    <t>ESP-nEN</t>
   </si>
 </sst>
 </file>
@@ -929,7 +929,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B32" s="1">
         <v>28</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B38" s="1">
         <v>34</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B39" s="1">
         <v>35</v>

</xml_diff>